<commit_message>
Extract data from sheets and created terminal interface
</commit_message>
<xml_diff>
--- a/tool_checkout_system.xlsx
+++ b/tool_checkout_system.xlsx
@@ -1,37 +1,124 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickpelletier/repos/barcode-checkout-system/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27862291-D9ED-084C-928B-4269FA5114A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="20080" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="tool_checkout_log" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="employees" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="tools" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="tool_checkout_log" sheetId="2" r:id="rId2"/>
+    <sheet name="employees" sheetId="3" r:id="rId3"/>
+    <sheet name="tools" sheetId="4" r:id="rId4"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
+  <si>
+    <t>Employee</t>
+  </si>
+  <si>
+    <t>Tool</t>
+  </si>
+  <si>
+    <t>Sign Out Time</t>
+  </si>
+  <si>
+    <t>Sing In Time</t>
+  </si>
+  <si>
+    <t>Employee Number</t>
+  </si>
+  <si>
+    <t>Employee Name</t>
+  </si>
+  <si>
+    <t>Tool Number</t>
+  </si>
+  <si>
+    <t>Tool Name</t>
+  </si>
+  <si>
+    <t>tool 1</t>
+  </si>
+  <si>
+    <t>tool 2</t>
+  </si>
+  <si>
+    <t>tool 3</t>
+  </si>
+  <si>
+    <t>tool 4</t>
+  </si>
+  <si>
+    <t>tool 5</t>
+  </si>
+  <si>
+    <t>tool 6</t>
+  </si>
+  <si>
+    <t>tool 7</t>
+  </si>
+  <si>
+    <t>tool 8</t>
+  </si>
+  <si>
+    <t>tool 9</t>
+  </si>
+  <si>
+    <t>tool 10</t>
+  </si>
+  <si>
+    <t>tool 11</t>
+  </si>
+  <si>
+    <t>tool 12</t>
+  </si>
+  <si>
+    <t>tool 13</t>
+  </si>
+  <si>
+    <t>tool 14</t>
+  </si>
+  <si>
+    <t>tool 15</t>
+  </si>
+  <si>
+    <t>john</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -50,80 +137,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -411,57 +439,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Employee</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Tool</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Sign Out Time</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Sing In Time</t>
-        </is>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -470,29 +478,144 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Employee Number</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Employee Name</t>
-        </is>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -501,32 +624,148 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Tool Number</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Tool Name</t>
-        </is>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Got sign out and sign in working.
</commit_message>
<xml_diff>
--- a/tool_checkout_system.xlsx
+++ b/tool_checkout_system.xlsx
@@ -433,21 +433,24 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col width="16.1640625" customWidth="1" min="3" max="3"/>
+    <col width="15.33203125" customWidth="1" min="1" max="1"/>
+    <col width="15.5" customWidth="1" min="3" max="3"/>
+    <col width="17.6640625" customWidth="1" min="4" max="4"/>
+    <col width="19.1640625" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Employee</t>
+          <t>Sign Out Employee</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -463,115 +466,92 @@
       <c r="D1" t="inlineStr">
         <is>
           <t>Sign In Time</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Sign In Employee</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>emp5</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>one</t>
+          <t>tool5</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>two</t>
+          <t>02/10/2024 14:03</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>02/10/2024 14:05</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>emp1</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>emp3</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>one</t>
+          <t>tool3</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>two</t>
+          <t>02/10/2024 14:04</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>02/10/2024 14:05</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>emp2</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>emp6</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>one</t>
+          <t>tool6</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>two</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>one</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>two</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>02/04/2024 18:58</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>emp1</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>tool1</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>02/04/2024 19:02</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>emp5</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>tool4</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>02/04/2024 19:03</t>
+          <t>02/10/2024 14:04</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>02/10/2024 14:05</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>emp6</t>
         </is>
       </c>
     </row>
@@ -586,13 +566,16 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col width="15.5" customWidth="1" min="1" max="1"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -703,56 +686,6 @@
       <c r="B11" t="inlineStr">
         <is>
           <t>emp10</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>emp11</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>12</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>emp12</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>13</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>emp13</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>14</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>emp14</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>15</v>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>emp15</t>
         </is>
       </c>
     </row>
@@ -767,10 +700,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B16"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -887,56 +820,6 @@
         </is>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>tool11</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>12</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>tool12</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>13</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>tool13</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>14</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>tool14</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>15</v>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>tool15</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add active tool functionality
</commit_message>
<xml_diff>
--- a/tool_checkout_system.xlsx
+++ b/tool_checkout_system.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="780" windowWidth="34200" windowHeight="20080" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="780" windowWidth="34200" windowHeight="20080" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
@@ -433,18 +433,16 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col width="15.33203125" customWidth="1" min="1" max="1"/>
-    <col width="15.5" customWidth="1" min="3" max="3"/>
-    <col width="17.6640625" customWidth="1" min="4" max="4"/>
-    <col width="19.1640625" customWidth="1" min="5" max="5"/>
+    <col width="16.83203125" customWidth="1" min="3" max="3"/>
+    <col width="16.6640625" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -477,22 +475,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>emp5</t>
+          <t>emp1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>tool5</t>
+          <t>tool1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>02/10/2024 14:03</t>
+          <t>02/10/2024 14:25</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>02/10/2024 14:05</t>
+          <t>02/10/2024 14:27</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -504,54 +502,240 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>emp3</t>
+          <t>emp2</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>tool3</t>
+          <t>tool2</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>02/10/2024 14:04</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>02/10/2024 14:05</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>emp2</t>
+          <t>02/10/2024 14:26</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>emp3</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>tool3</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>02/10/2024 14:26</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>02/10/2024 14:40</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>emp3</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>emp4</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>tool4</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>02/10/2024 14:26</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>02/10/2024 14:27</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>emp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>emp5</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>tool5</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>02/10/2024 14:26</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>02/10/2024 14:37</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>emp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
           <t>emp6</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B7" t="inlineStr">
         <is>
           <t>tool6</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>02/10/2024 14:04</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>02/10/2024 14:05</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>02/10/2024 14:26</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>02/10/2024 14:39</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
         <is>
           <t>emp6</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>emp7</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>tool7</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>02/10/2024 14:26</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>02/10/2024 14:27</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>emp7</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>emp8</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>tool8</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>02/10/2024 14:26</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>02/10/2024 14:27</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>emp8</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>emp9</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>tool9</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>02/10/2024 14:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>emp5</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>tool5</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>02/10/2024 14:39</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>02/10/2024 14:43</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>emp5</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>emp7</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>tool7</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>02/10/2024 14:40</t>
         </is>
       </c>
     </row>
@@ -569,13 +753,10 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="B2" sqref="B2:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
-  <cols>
-    <col width="15.5" customWidth="1" min="1" max="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -700,10 +881,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -719,6 +900,11 @@
           <t>Tool Name</t>
         </is>
       </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -739,6 +925,11 @@
           <t>tool2</t>
         </is>
       </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -789,6 +980,11 @@
           <t>tool7</t>
         </is>
       </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -807,6 +1003,11 @@
       <c r="B10" t="inlineStr">
         <is>
           <t>tool9</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Active</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added data entry script to easily enter tools and employees
</commit_message>
<xml_diff>
--- a/tool_checkout_system.xlsx
+++ b/tool_checkout_system.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="780" windowWidth="34200" windowHeight="20080" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="780" windowWidth="34200" windowHeight="20080" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="tool_checkout_log" sheetId="1" state="visible" r:id="rId1"/>
@@ -18,18 +18,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <sz val="8"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -420,9 +414,9 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -530,6 +524,16 @@
           <t>02/10/2024 14:56</t>
         </is>
       </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>02/10/2024 18:50</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>joe</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -582,6 +586,33 @@
       <c r="E6" t="inlineStr">
         <is>
           <t>emp5</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>joe</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>screw</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>02/10/2024 18:49</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>02/10/2024 18:49</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>joe</t>
         </is>
       </c>
     </row>
@@ -596,7 +627,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B11"/>
@@ -719,6 +750,16 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>1234</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>joe</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -730,10 +771,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -784,11 +825,6 @@
           <t>tool3</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Active</t>
-        </is>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -857,6 +893,26 @@
       <c r="B11" t="inlineStr">
         <is>
           <t>tool10</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>14543</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>hammer</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12345</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>screw</t>
         </is>
       </c>
     </row>

</xml_diff>